<commit_message>
Added city name to the query
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="46">
   <si>
     <t xml:space="preserve">Retailer name</t>
   </si>
@@ -152,6 +152,12 @@
   </si>
   <si>
     <t xml:space="preserve">DHANCHOWMUHANI,RANIR BAZAR,AGARTALA,(W)TRIPURA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAKSHI MOTORS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mayapuri</t>
   </si>
 </sst>
 </file>
@@ -265,19 +271,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="79.8016194331984"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="173.425101214575"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.6761133603239"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.9514170040486"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="80.4453441295547"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="175.032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.3805668016194"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.7813765182186"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -562,6 +568,14 @@
       </c>
       <c r="D20" s="2" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change in retailer name lookup
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="49">
   <si>
     <t xml:space="preserve">Retailer name</t>
   </si>
@@ -158,6 +158,15 @@
   </si>
   <si>
     <t xml:space="preserve">Mayapuri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALLIED AGENCY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ahmedabad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aeroflon Engineers Pvt Ltd.</t>
   </si>
 </sst>
 </file>
@@ -271,19 +280,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="80.4453441295547"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="175.032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.7813765182186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.3805668016194"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="81.1943319838057"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="176.63967611336"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.7044534412956"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.8906882591093"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -576,6 +585,22 @@
       </c>
       <c r="C21" s="0" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>